<commit_message>
Added Log. Reg. for GDP
</commit_message>
<xml_diff>
--- a/data/GFK-konsumklima-index-monatlich.xlsx
+++ b/data/GFK-konsumklima-index-monatlich.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masterarbeit-WebScraper\WebScraper\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masterthesis\WebScraper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EC43A1-5964-40E5-9327-E55D837D7BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967BEE36-A250-436A-9C98-78F654AABCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
     <sheet name="Daten" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -410,33 +423,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>GfK-Konsumklima</a:t>
+              <a:t>GfK-Konsumklima-Index</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t>-Index</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -453,25 +455,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -497,46 +493,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="100000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="130000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="50000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="350000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="16200000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="35000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-            <a:scene3d>
-              <a:camera prst="orthographicFront">
-                <a:rot lat="0" lon="0" rev="0"/>
-              </a:camera>
-              <a:lightRig rig="threePt" dir="t">
-                <a:rot lat="0" lon="0" rev="1200000"/>
-              </a:lightRig>
-            </a:scene3d>
-            <a:sp3d>
-              <a:bevelT w="63500" h="25400"/>
-            </a:sp3d>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -840,8 +803,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
+        <c:gapWidth val="199"/>
         <c:axId val="529464575"/>
         <c:axId val="529455839"/>
       </c:barChart>
@@ -858,11 +820,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -874,10 +836,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -885,7 +848,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="529455839"/>
@@ -906,9 +869,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -916,6 +879,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -934,8 +911,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -943,7 +921,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="529464575"/>
@@ -963,28 +941,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -995,7 +962,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1047,41 +1014,43 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1089,36 +1058,29 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1129,13 +1091,16 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1145,35 +1110,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="38100" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1182,34 +1157,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1225,16 +1195,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1246,7 +1217,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1257,9 +1228,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1270,14 +1241,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -1289,13 +1260,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1307,7 +1279,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -1315,14 +1287,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1334,16 +1306,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1352,14 +1325,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -1371,14 +1344,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1389,26 +1362,27 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1416,16 +1390,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1438,14 +1413,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1456,20 +1431,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1478,13 +1446,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1493,8 +1462,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1504,7 +1474,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1512,9 +1482,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1525,8 +1495,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1536,7 +1507,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -1907,28 +1878,28 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="3" width="70.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1936,7 +1907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E9" s="11" t="s">
         <v>20</v>
       </c>
@@ -1946,7 +1917,7 @@
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1960,7 +1931,7 @@
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1945,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1988,7 +1959,7 @@
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2002,7 +1973,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -2016,7 +1987,7 @@
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2030,7 +2001,7 @@
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2044,7 +2015,7 @@
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2058,7 +2029,7 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" ht="25" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -2072,7 +2043,7 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -2080,7 +2051,7 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2091,7 +2062,7 @@
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -2099,7 +2070,7 @@
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2113,7 +2084,7 @@
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
@@ -2127,7 +2098,7 @@
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
@@ -2141,7 +2112,7 @@
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
@@ -2155,7 +2126,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -2163,7 +2134,7 @@
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -2171,7 +2142,7 @@
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
@@ -2179,7 +2150,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -2187,7 +2158,7 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -2195,7 +2166,7 @@
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -2203,7 +2174,7 @@
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
@@ -2211,7 +2182,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
@@ -2219,7 +2190,7 @@
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
     </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
@@ -2227,7 +2198,7 @@
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
@@ -2235,7 +2206,7 @@
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
     </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -2243,7 +2214,7 @@
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
     </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -2251,7 +2222,7 @@
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
     </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
@@ -2259,7 +2230,7 @@
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
     </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
@@ -2267,7 +2238,7 @@
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
     </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -2275,7 +2246,7 @@
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
     </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
@@ -2283,7 +2254,7 @@
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
     </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
@@ -2291,7 +2262,7 @@
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
     </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
@@ -2299,7 +2270,7 @@
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
     </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
@@ -2307,7 +2278,7 @@
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -2315,7 +2286,7 @@
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
@@ -2323,7 +2294,7 @@
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
@@ -2331,7 +2302,7 @@
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
     </row>
-    <row r="48" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
@@ -2339,7 +2310,7 @@
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
     </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
@@ -2347,7 +2318,7 @@
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
     </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
@@ -2355,7 +2326,7 @@
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
     </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
@@ -2363,7 +2334,7 @@
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
     </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -2371,7 +2342,7 @@
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
     </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
@@ -2379,7 +2350,7 @@
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
     </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
@@ -2387,7 +2358,7 @@
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
@@ -2395,7 +2366,7 @@
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
     </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
@@ -2403,7 +2374,7 @@
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
     </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
@@ -2411,7 +2382,7 @@
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
     </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
@@ -2419,7 +2390,7 @@
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
     </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
@@ -2427,7 +2398,7 @@
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
     </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
@@ -2435,7 +2406,7 @@
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
     </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
@@ -2443,7 +2414,7 @@
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
     </row>
-    <row r="62" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
@@ -2451,7 +2422,7 @@
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
     </row>
-    <row r="63" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
@@ -2459,7 +2430,7 @@
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
     </row>
-    <row r="64" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
@@ -2467,7 +2438,7 @@
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
     </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
@@ -2475,7 +2446,7 @@
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
     </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
@@ -2483,7 +2454,7 @@
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
     </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
@@ -2491,7 +2462,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
     </row>
-    <row r="68" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
@@ -2499,7 +2470,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
     </row>
-    <row r="69" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
@@ -2507,7 +2478,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
     </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E70" s="12"/>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
@@ -2515,7 +2486,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
     </row>
-    <row r="71" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
@@ -2523,7 +2494,7 @@
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
     </row>
-    <row r="72" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E72" s="12"/>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
@@ -2531,7 +2502,7 @@
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
     </row>
-    <row r="73" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
@@ -2539,7 +2510,7 @@
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
     </row>
-    <row r="74" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E74" s="12"/>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
@@ -2547,7 +2518,7 @@
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
     </row>
-    <row r="75" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E75" s="12"/>
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
@@ -2555,7 +2526,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
     </row>
-    <row r="76" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E76" s="12"/>
       <c r="F76" s="12"/>
       <c r="G76" s="12"/>
@@ -2563,7 +2534,7 @@
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
     </row>
-    <row r="77" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E77" s="12"/>
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
@@ -2571,7 +2542,7 @@
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
     </row>
-    <row r="78" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E78" s="12"/>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
@@ -2579,7 +2550,7 @@
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
     </row>
-    <row r="79" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
@@ -2587,7 +2558,7 @@
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
     </row>
-    <row r="80" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E80" s="12"/>
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
@@ -2595,7 +2566,7 @@
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
     </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E81" s="12"/>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
@@ -2603,7 +2574,7 @@
       <c r="I81" s="12"/>
       <c r="J81" s="12"/>
     </row>
-    <row r="82" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E82" s="12"/>
       <c r="F82" s="12"/>
       <c r="G82" s="12"/>
@@ -2611,7 +2582,7 @@
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
     </row>
-    <row r="83" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
@@ -2619,7 +2590,7 @@
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
     </row>
-    <row r="84" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
@@ -2627,7 +2598,7 @@
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
     </row>
-    <row r="85" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
@@ -2635,7 +2606,7 @@
       <c r="I85" s="12"/>
       <c r="J85" s="12"/>
     </row>
-    <row r="86" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
@@ -2643,7 +2614,7 @@
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
     </row>
-    <row r="87" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
@@ -2651,7 +2622,7 @@
       <c r="I87" s="12"/>
       <c r="J87" s="12"/>
     </row>
-    <row r="88" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
@@ -2659,7 +2630,7 @@
       <c r="I88" s="12"/>
       <c r="J88" s="12"/>
     </row>
-    <row r="89" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E89" s="12"/>
       <c r="F89" s="12"/>
       <c r="G89" s="12"/>
@@ -2667,7 +2638,7 @@
       <c r="I89" s="12"/>
       <c r="J89" s="12"/>
     </row>
-    <row r="90" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -2675,7 +2646,7 @@
       <c r="I90" s="12"/>
       <c r="J90" s="12"/>
     </row>
-    <row r="91" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E91" s="12"/>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
@@ -2683,7 +2654,7 @@
       <c r="I91" s="12"/>
       <c r="J91" s="12"/>
     </row>
-    <row r="92" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
@@ -2691,7 +2662,7 @@
       <c r="I92" s="12"/>
       <c r="J92" s="12"/>
     </row>
-    <row r="93" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E93" s="12"/>
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
@@ -2699,7 +2670,7 @@
       <c r="I93" s="12"/>
       <c r="J93" s="12"/>
     </row>
-    <row r="94" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
@@ -2707,7 +2678,7 @@
       <c r="I94" s="12"/>
       <c r="J94" s="12"/>
     </row>
-    <row r="95" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E95" s="12"/>
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
@@ -2715,7 +2686,7 @@
       <c r="I95" s="12"/>
       <c r="J95" s="12"/>
     </row>
-    <row r="96" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E96" s="12"/>
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
@@ -2723,7 +2694,7 @@
       <c r="I96" s="12"/>
       <c r="J96" s="12"/>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E97" s="12"/>
       <c r="F97" s="12"/>
       <c r="G97" s="12"/>
@@ -2731,7 +2702,7 @@
       <c r="I97" s="12"/>
       <c r="J97" s="12"/>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E98" s="12"/>
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
@@ -2739,7 +2710,7 @@
       <c r="I98" s="12"/>
       <c r="J98" s="12"/>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
@@ -2747,7 +2718,7 @@
       <c r="I99" s="12"/>
       <c r="J99" s="12"/>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
@@ -2755,7 +2726,7 @@
       <c r="I100" s="12"/>
       <c r="J100" s="12"/>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
@@ -2763,7 +2734,7 @@
       <c r="I101" s="12"/>
       <c r="J101" s="12"/>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
@@ -2771,7 +2742,7 @@
       <c r="I102" s="12"/>
       <c r="J102" s="12"/>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
@@ -2779,7 +2750,7 @@
       <c r="I103" s="12"/>
       <c r="J103" s="12"/>
     </row>
-    <row r="104" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E104" s="12"/>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
@@ -2787,7 +2758,7 @@
       <c r="I104" s="12"/>
       <c r="J104" s="12"/>
     </row>
-    <row r="105" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E105" s="12"/>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
@@ -2795,7 +2766,7 @@
       <c r="I105" s="12"/>
       <c r="J105" s="12"/>
     </row>
-    <row r="106" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
@@ -2803,7 +2774,7 @@
       <c r="I106" s="12"/>
       <c r="J106" s="12"/>
     </row>
-    <row r="107" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E107" s="12"/>
       <c r="F107" s="12"/>
       <c r="G107" s="12"/>
@@ -2811,7 +2782,7 @@
       <c r="I107" s="12"/>
       <c r="J107" s="12"/>
     </row>
-    <row r="108" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E108" s="12"/>
       <c r="F108" s="12"/>
       <c r="G108" s="12"/>
@@ -2819,7 +2790,7 @@
       <c r="I108" s="12"/>
       <c r="J108" s="12"/>
     </row>
-    <row r="109" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E109" s="12"/>
       <c r="F109" s="12"/>
       <c r="G109" s="12"/>
@@ -2827,7 +2798,7 @@
       <c r="I109" s="12"/>
       <c r="J109" s="12"/>
     </row>
-    <row r="110" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E110" s="12"/>
       <c r="F110" s="12"/>
       <c r="G110" s="12"/>
@@ -2835,7 +2806,7 @@
       <c r="I110" s="12"/>
       <c r="J110" s="12"/>
     </row>
-    <row r="111" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E111" s="12"/>
       <c r="F111" s="12"/>
       <c r="G111" s="12"/>
@@ -2843,7 +2814,7 @@
       <c r="I111" s="12"/>
       <c r="J111" s="12"/>
     </row>
-    <row r="112" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E112" s="12"/>
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
@@ -2851,7 +2822,7 @@
       <c r="I112" s="12"/>
       <c r="J112" s="12"/>
     </row>
-    <row r="113" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E113" s="12"/>
       <c r="F113" s="12"/>
       <c r="G113" s="12"/>
@@ -2859,7 +2830,7 @@
       <c r="I113" s="12"/>
       <c r="J113" s="12"/>
     </row>
-    <row r="114" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E114" s="12"/>
       <c r="F114" s="12"/>
       <c r="G114" s="12"/>
@@ -2867,7 +2838,7 @@
       <c r="I114" s="12"/>
       <c r="J114" s="12"/>
     </row>
-    <row r="115" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E115" s="12"/>
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
@@ -2875,7 +2846,7 @@
       <c r="I115" s="12"/>
       <c r="J115" s="12"/>
     </row>
-    <row r="116" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E116" s="12"/>
       <c r="F116" s="12"/>
       <c r="G116" s="12"/>
@@ -2883,7 +2854,7 @@
       <c r="I116" s="12"/>
       <c r="J116" s="12"/>
     </row>
-    <row r="117" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
       <c r="G117" s="12"/>
@@ -2891,7 +2862,7 @@
       <c r="I117" s="12"/>
       <c r="J117" s="12"/>
     </row>
-    <row r="118" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E118" s="12"/>
       <c r="F118" s="12"/>
       <c r="G118" s="12"/>
@@ -2899,7 +2870,7 @@
       <c r="I118" s="12"/>
       <c r="J118" s="12"/>
     </row>
-    <row r="119" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E119" s="12"/>
       <c r="F119" s="12"/>
       <c r="G119" s="12"/>
@@ -2907,7 +2878,7 @@
       <c r="I119" s="12"/>
       <c r="J119" s="12"/>
     </row>
-    <row r="120" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E120" s="12"/>
       <c r="F120" s="12"/>
       <c r="G120" s="12"/>
@@ -2915,7 +2886,7 @@
       <c r="I120" s="12"/>
       <c r="J120" s="12"/>
     </row>
-    <row r="121" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E121" s="12"/>
       <c r="F121" s="12"/>
       <c r="G121" s="12"/>
@@ -2923,7 +2894,7 @@
       <c r="I121" s="12"/>
       <c r="J121" s="12"/>
     </row>
-    <row r="122" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
       <c r="G122" s="12"/>
@@ -2931,7 +2902,7 @@
       <c r="I122" s="12"/>
       <c r="J122" s="12"/>
     </row>
-    <row r="123" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E123" s="12"/>
       <c r="F123" s="12"/>
       <c r="G123" s="12"/>
@@ -2939,7 +2910,7 @@
       <c r="I123" s="12"/>
       <c r="J123" s="12"/>
     </row>
-    <row r="124" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E124" s="12"/>
       <c r="F124" s="12"/>
       <c r="G124" s="12"/>
@@ -2947,7 +2918,7 @@
       <c r="I124" s="12"/>
       <c r="J124" s="12"/>
     </row>
-    <row r="125" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E125" s="12"/>
       <c r="F125" s="12"/>
       <c r="G125" s="12"/>
@@ -2955,7 +2926,7 @@
       <c r="I125" s="12"/>
       <c r="J125" s="12"/>
     </row>
-    <row r="126" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E126" s="12"/>
       <c r="F126" s="12"/>
       <c r="G126" s="12"/>
@@ -2963,7 +2934,7 @@
       <c r="I126" s="12"/>
       <c r="J126" s="12"/>
     </row>
-    <row r="127" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
       <c r="G127" s="12"/>
@@ -2971,7 +2942,7 @@
       <c r="I127" s="12"/>
       <c r="J127" s="12"/>
     </row>
-    <row r="128" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E128" s="12"/>
       <c r="F128" s="12"/>
       <c r="G128" s="12"/>
@@ -2979,7 +2950,7 @@
       <c r="I128" s="12"/>
       <c r="J128" s="12"/>
     </row>
-    <row r="129" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E129" s="12"/>
       <c r="F129" s="12"/>
       <c r="G129" s="12"/>
@@ -2987,7 +2958,7 @@
       <c r="I129" s="12"/>
       <c r="J129" s="12"/>
     </row>
-    <row r="130" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E130" s="12"/>
       <c r="F130" s="12"/>
       <c r="G130" s="12"/>
@@ -2995,7 +2966,7 @@
       <c r="I130" s="12"/>
       <c r="J130" s="12"/>
     </row>
-    <row r="131" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E131" s="12"/>
       <c r="F131" s="12"/>
       <c r="G131" s="12"/>
@@ -3003,7 +2974,7 @@
       <c r="I131" s="12"/>
       <c r="J131" s="12"/>
     </row>
-    <row r="132" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E132" s="12"/>
       <c r="F132" s="12"/>
       <c r="G132" s="12"/>
@@ -3011,7 +2982,7 @@
       <c r="I132" s="12"/>
       <c r="J132" s="12"/>
     </row>
-    <row r="133" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E133" s="12"/>
       <c r="F133" s="12"/>
       <c r="G133" s="12"/>
@@ -3019,7 +2990,7 @@
       <c r="I133" s="12"/>
       <c r="J133" s="12"/>
     </row>
-    <row r="134" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E134" s="12"/>
       <c r="F134" s="12"/>
       <c r="G134" s="12"/>
@@ -3027,7 +2998,7 @@
       <c r="I134" s="12"/>
       <c r="J134" s="12"/>
     </row>
-    <row r="135" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E135" s="12"/>
       <c r="F135" s="12"/>
       <c r="G135" s="12"/>
@@ -3035,7 +3006,7 @@
       <c r="I135" s="12"/>
       <c r="J135" s="12"/>
     </row>
-    <row r="136" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E136" s="12"/>
       <c r="F136" s="12"/>
       <c r="G136" s="12"/>
@@ -3043,7 +3014,7 @@
       <c r="I136" s="12"/>
       <c r="J136" s="12"/>
     </row>
-    <row r="137" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E137" s="12"/>
       <c r="F137" s="12"/>
       <c r="G137" s="12"/>
@@ -3051,7 +3022,7 @@
       <c r="I137" s="12"/>
       <c r="J137" s="12"/>
     </row>
-    <row r="138" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
       <c r="G138" s="12"/>
@@ -3059,7 +3030,7 @@
       <c r="I138" s="12"/>
       <c r="J138" s="12"/>
     </row>
-    <row r="139" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E139" s="12"/>
       <c r="F139" s="12"/>
       <c r="G139" s="12"/>
@@ -3067,7 +3038,7 @@
       <c r="I139" s="12"/>
       <c r="J139" s="12"/>
     </row>
-    <row r="140" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
       <c r="G140" s="12"/>
@@ -3075,7 +3046,7 @@
       <c r="I140" s="12"/>
       <c r="J140" s="12"/>
     </row>
-    <row r="141" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E141" s="12"/>
       <c r="F141" s="12"/>
       <c r="G141" s="12"/>
@@ -3083,7 +3054,7 @@
       <c r="I141" s="12"/>
       <c r="J141" s="12"/>
     </row>
-    <row r="142" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E142" s="12"/>
       <c r="F142" s="12"/>
       <c r="G142" s="12"/>
@@ -3091,7 +3062,7 @@
       <c r="I142" s="12"/>
       <c r="J142" s="12"/>
     </row>
-    <row r="143" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E143" s="12"/>
       <c r="F143" s="12"/>
       <c r="G143" s="12"/>
@@ -3099,7 +3070,7 @@
       <c r="I143" s="12"/>
       <c r="J143" s="12"/>
     </row>
-    <row r="144" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E144" s="12"/>
       <c r="F144" s="12"/>
       <c r="G144" s="12"/>
@@ -3107,7 +3078,7 @@
       <c r="I144" s="12"/>
       <c r="J144" s="12"/>
     </row>
-    <row r="145" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E145" s="12"/>
       <c r="F145" s="12"/>
       <c r="G145" s="12"/>
@@ -3115,7 +3086,7 @@
       <c r="I145" s="12"/>
       <c r="J145" s="12"/>
     </row>
-    <row r="146" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E146" s="12"/>
       <c r="F146" s="12"/>
       <c r="G146" s="12"/>
@@ -3123,7 +3094,7 @@
       <c r="I146" s="12"/>
       <c r="J146" s="12"/>
     </row>
-    <row r="147" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E147" s="12"/>
       <c r="F147" s="12"/>
       <c r="G147" s="12"/>
@@ -3131,7 +3102,7 @@
       <c r="I147" s="12"/>
       <c r="J147" s="12"/>
     </row>
-    <row r="148" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E148" s="12"/>
       <c r="F148" s="12"/>
       <c r="G148" s="12"/>
@@ -3139,7 +3110,7 @@
       <c r="I148" s="12"/>
       <c r="J148" s="12"/>
     </row>
-    <row r="149" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E149" s="12"/>
       <c r="F149" s="12"/>
       <c r="G149" s="12"/>
@@ -3147,7 +3118,7 @@
       <c r="I149" s="12"/>
       <c r="J149" s="12"/>
     </row>
-    <row r="150" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E150" s="12"/>
       <c r="F150" s="12"/>
       <c r="G150" s="12"/>
@@ -3155,7 +3126,7 @@
       <c r="I150" s="12"/>
       <c r="J150" s="12"/>
     </row>
-    <row r="151" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E151" s="12"/>
       <c r="F151" s="12"/>
       <c r="G151" s="12"/>
@@ -3163,7 +3134,7 @@
       <c r="I151" s="12"/>
       <c r="J151" s="12"/>
     </row>
-    <row r="152" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E152" s="12"/>
       <c r="F152" s="12"/>
       <c r="G152" s="12"/>
@@ -3171,7 +3142,7 @@
       <c r="I152" s="12"/>
       <c r="J152" s="12"/>
     </row>
-    <row r="153" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E153" s="12"/>
       <c r="F153" s="12"/>
       <c r="G153" s="12"/>
@@ -3179,7 +3150,7 @@
       <c r="I153" s="12"/>
       <c r="J153" s="12"/>
     </row>
-    <row r="154" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E154" s="12"/>
       <c r="F154" s="12"/>
       <c r="G154" s="12"/>
@@ -3187,7 +3158,7 @@
       <c r="I154" s="12"/>
       <c r="J154" s="12"/>
     </row>
-    <row r="155" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E155" s="12"/>
       <c r="F155" s="12"/>
       <c r="G155" s="12"/>
@@ -3195,7 +3166,7 @@
       <c r="I155" s="12"/>
       <c r="J155" s="12"/>
     </row>
-    <row r="156" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E156" s="12"/>
       <c r="F156" s="12"/>
       <c r="G156" s="12"/>
@@ -3203,7 +3174,7 @@
       <c r="I156" s="12"/>
       <c r="J156" s="12"/>
     </row>
-    <row r="157" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E157" s="12"/>
       <c r="F157" s="12"/>
       <c r="G157" s="12"/>
@@ -3211,7 +3182,7 @@
       <c r="I157" s="12"/>
       <c r="J157" s="12"/>
     </row>
-    <row r="158" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E158" s="12"/>
       <c r="F158" s="12"/>
       <c r="G158" s="12"/>
@@ -3219,7 +3190,7 @@
       <c r="I158" s="12"/>
       <c r="J158" s="12"/>
     </row>
-    <row r="159" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E159" s="12"/>
       <c r="F159" s="12"/>
       <c r="G159" s="12"/>
@@ -3227,7 +3198,7 @@
       <c r="I159" s="12"/>
       <c r="J159" s="12"/>
     </row>
-    <row r="160" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E160" s="12"/>
       <c r="F160" s="12"/>
       <c r="G160" s="12"/>
@@ -3235,7 +3206,7 @@
       <c r="I160" s="12"/>
       <c r="J160" s="12"/>
     </row>
-    <row r="161" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
       <c r="G161" s="12"/>
@@ -3243,7 +3214,7 @@
       <c r="I161" s="12"/>
       <c r="J161" s="12"/>
     </row>
-    <row r="162" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E162" s="12"/>
       <c r="F162" s="12"/>
       <c r="G162" s="12"/>
@@ -3251,7 +3222,7 @@
       <c r="I162" s="12"/>
       <c r="J162" s="12"/>
     </row>
-    <row r="163" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E163" s="12"/>
       <c r="F163" s="12"/>
       <c r="G163" s="12"/>
@@ -3259,7 +3230,7 @@
       <c r="I163" s="12"/>
       <c r="J163" s="12"/>
     </row>
-    <row r="164" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E164" s="12"/>
       <c r="F164" s="12"/>
       <c r="G164" s="12"/>
@@ -3267,7 +3238,7 @@
       <c r="I164" s="12"/>
       <c r="J164" s="12"/>
     </row>
-    <row r="165" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E165" s="12"/>
       <c r="F165" s="12"/>
       <c r="G165" s="12"/>
@@ -3275,7 +3246,7 @@
       <c r="I165" s="12"/>
       <c r="J165" s="12"/>
     </row>
-    <row r="166" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E166" s="12"/>
       <c r="F166" s="12"/>
       <c r="G166" s="12"/>
@@ -3283,7 +3254,7 @@
       <c r="I166" s="12"/>
       <c r="J166" s="12"/>
     </row>
-    <row r="167" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
       <c r="G167" s="12"/>
@@ -3291,7 +3262,7 @@
       <c r="I167" s="12"/>
       <c r="J167" s="12"/>
     </row>
-    <row r="168" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E168" s="12"/>
       <c r="F168" s="12"/>
       <c r="G168" s="12"/>
@@ -3299,7 +3270,7 @@
       <c r="I168" s="12"/>
       <c r="J168" s="12"/>
     </row>
-    <row r="169" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E169" s="12"/>
       <c r="F169" s="12"/>
       <c r="G169" s="12"/>
@@ -3307,7 +3278,7 @@
       <c r="I169" s="12"/>
       <c r="J169" s="12"/>
     </row>
-    <row r="170" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E170" s="12"/>
       <c r="F170" s="12"/>
       <c r="G170" s="12"/>
@@ -3315,7 +3286,7 @@
       <c r="I170" s="12"/>
       <c r="J170" s="12"/>
     </row>
-    <row r="171" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E171" s="12"/>
       <c r="F171" s="12"/>
       <c r="G171" s="12"/>
@@ -3323,7 +3294,7 @@
       <c r="I171" s="12"/>
       <c r="J171" s="12"/>
     </row>
-    <row r="172" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E172" s="12"/>
       <c r="F172" s="12"/>
       <c r="G172" s="12"/>
@@ -3331,7 +3302,7 @@
       <c r="I172" s="12"/>
       <c r="J172" s="12"/>
     </row>
-    <row r="173" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E173" s="12"/>
       <c r="F173" s="12"/>
       <c r="G173" s="12"/>
@@ -3339,7 +3310,7 @@
       <c r="I173" s="12"/>
       <c r="J173" s="12"/>
     </row>
-    <row r="174" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E174" s="12"/>
       <c r="F174" s="12"/>
       <c r="G174" s="12"/>
@@ -3347,7 +3318,7 @@
       <c r="I174" s="12"/>
       <c r="J174" s="12"/>
     </row>
-    <row r="175" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E175" s="12"/>
       <c r="F175" s="12"/>
       <c r="G175" s="12"/>
@@ -3355,7 +3326,7 @@
       <c r="I175" s="12"/>
       <c r="J175" s="12"/>
     </row>
-    <row r="176" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E176" s="12"/>
       <c r="F176" s="12"/>
       <c r="G176" s="12"/>
@@ -3363,7 +3334,7 @@
       <c r="I176" s="12"/>
       <c r="J176" s="12"/>
     </row>
-    <row r="177" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E177" s="12"/>
       <c r="F177" s="12"/>
       <c r="G177" s="12"/>
@@ -3371,7 +3342,7 @@
       <c r="I177" s="12"/>
       <c r="J177" s="12"/>
     </row>
-    <row r="178" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E178" s="12"/>
       <c r="F178" s="12"/>
       <c r="G178" s="12"/>
@@ -3379,7 +3350,7 @@
       <c r="I178" s="12"/>
       <c r="J178" s="12"/>
     </row>
-    <row r="179" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E179" s="12"/>
       <c r="F179" s="12"/>
       <c r="G179" s="12"/>
@@ -3387,7 +3358,7 @@
       <c r="I179" s="12"/>
       <c r="J179" s="12"/>
     </row>
-    <row r="180" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E180" s="12"/>
       <c r="F180" s="12"/>
       <c r="G180" s="12"/>
@@ -3395,7 +3366,7 @@
       <c r="I180" s="12"/>
       <c r="J180" s="12"/>
     </row>
-    <row r="181" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E181" s="12"/>
       <c r="F181" s="12"/>
       <c r="G181" s="12"/>
@@ -3403,7 +3374,7 @@
       <c r="I181" s="12"/>
       <c r="J181" s="12"/>
     </row>
-    <row r="182" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E182" s="12"/>
       <c r="F182" s="12"/>
       <c r="G182" s="12"/>
@@ -3411,7 +3382,7 @@
       <c r="I182" s="12"/>
       <c r="J182" s="12"/>
     </row>
-    <row r="183" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E183" s="12"/>
       <c r="F183" s="12"/>
       <c r="G183" s="12"/>
@@ -3419,7 +3390,7 @@
       <c r="I183" s="12"/>
       <c r="J183" s="12"/>
     </row>
-    <row r="184" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E184" s="12"/>
       <c r="F184" s="12"/>
       <c r="G184" s="12"/>
@@ -3427,7 +3398,7 @@
       <c r="I184" s="12"/>
       <c r="J184" s="12"/>
     </row>
-    <row r="185" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
       <c r="G185" s="12"/>
@@ -3435,7 +3406,7 @@
       <c r="I185" s="12"/>
       <c r="J185" s="12"/>
     </row>
-    <row r="186" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E186" s="12"/>
       <c r="F186" s="12"/>
       <c r="G186" s="12"/>
@@ -3443,7 +3414,7 @@
       <c r="I186" s="12"/>
       <c r="J186" s="12"/>
     </row>
-    <row r="187" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E187" s="12"/>
       <c r="F187" s="12"/>
       <c r="G187" s="12"/>
@@ -3451,7 +3422,7 @@
       <c r="I187" s="12"/>
       <c r="J187" s="12"/>
     </row>
-    <row r="188" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E188" s="12"/>
       <c r="F188" s="12"/>
       <c r="G188" s="12"/>
@@ -3459,7 +3430,7 @@
       <c r="I188" s="12"/>
       <c r="J188" s="12"/>
     </row>
-    <row r="189" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E189" s="12"/>
       <c r="F189" s="12"/>
       <c r="G189" s="12"/>
@@ -3467,7 +3438,7 @@
       <c r="I189" s="12"/>
       <c r="J189" s="12"/>
     </row>
-    <row r="190" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E190" s="12"/>
       <c r="F190" s="12"/>
       <c r="G190" s="12"/>
@@ -3475,7 +3446,7 @@
       <c r="I190" s="12"/>
       <c r="J190" s="12"/>
     </row>
-    <row r="191" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E191" s="12"/>
       <c r="F191" s="12"/>
       <c r="G191" s="12"/>
@@ -3483,7 +3454,7 @@
       <c r="I191" s="12"/>
       <c r="J191" s="12"/>
     </row>
-    <row r="192" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E192" s="12"/>
       <c r="F192" s="12"/>
       <c r="G192" s="12"/>
@@ -3491,7 +3462,7 @@
       <c r="I192" s="12"/>
       <c r="J192" s="12"/>
     </row>
-    <row r="193" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E193" s="12"/>
       <c r="F193" s="12"/>
       <c r="G193" s="12"/>
@@ -3499,7 +3470,7 @@
       <c r="I193" s="12"/>
       <c r="J193" s="12"/>
     </row>
-    <row r="194" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E194" s="12"/>
       <c r="F194" s="12"/>
       <c r="G194" s="12"/>
@@ -3507,7 +3478,7 @@
       <c r="I194" s="12"/>
       <c r="J194" s="12"/>
     </row>
-    <row r="195" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E195" s="12"/>
       <c r="F195" s="12"/>
       <c r="G195" s="12"/>
@@ -3515,7 +3486,7 @@
       <c r="I195" s="12"/>
       <c r="J195" s="12"/>
     </row>
-    <row r="196" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E196" s="12"/>
       <c r="F196" s="12"/>
       <c r="G196" s="12"/>
@@ -3523,7 +3494,7 @@
       <c r="I196" s="12"/>
       <c r="J196" s="12"/>
     </row>
-    <row r="197" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E197" s="12"/>
       <c r="F197" s="12"/>
       <c r="G197" s="12"/>
@@ -3531,7 +3502,7 @@
       <c r="I197" s="12"/>
       <c r="J197" s="12"/>
     </row>
-    <row r="198" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E198" s="12"/>
       <c r="F198" s="12"/>
       <c r="G198" s="12"/>
@@ -3539,7 +3510,7 @@
       <c r="I198" s="12"/>
       <c r="J198" s="12"/>
     </row>
-    <row r="199" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E199" s="12"/>
       <c r="F199" s="12"/>
       <c r="G199" s="12"/>
@@ -3547,7 +3518,7 @@
       <c r="I199" s="12"/>
       <c r="J199" s="12"/>
     </row>
-    <row r="200" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E200" s="12"/>
       <c r="F200" s="12"/>
       <c r="G200" s="12"/>
@@ -3555,7 +3526,7 @@
       <c r="I200" s="12"/>
       <c r="J200" s="12"/>
     </row>
-    <row r="201" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E201" s="12"/>
       <c r="F201" s="12"/>
       <c r="G201" s="12"/>
@@ -3563,7 +3534,7 @@
       <c r="I201" s="12"/>
       <c r="J201" s="12"/>
     </row>
-    <row r="202" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E202" s="12"/>
       <c r="F202" s="12"/>
       <c r="G202" s="12"/>
@@ -3571,7 +3542,7 @@
       <c r="I202" s="12"/>
       <c r="J202" s="12"/>
     </row>
-    <row r="203" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E203" s="12"/>
       <c r="F203" s="12"/>
       <c r="G203" s="12"/>
@@ -3579,7 +3550,7 @@
       <c r="I203" s="12"/>
       <c r="J203" s="12"/>
     </row>
-    <row r="204" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
       <c r="G204" s="12"/>
@@ -3587,7 +3558,7 @@
       <c r="I204" s="12"/>
       <c r="J204" s="12"/>
     </row>
-    <row r="205" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E205" s="12"/>
       <c r="F205" s="12"/>
       <c r="G205" s="12"/>
@@ -3595,7 +3566,7 @@
       <c r="I205" s="12"/>
       <c r="J205" s="12"/>
     </row>
-    <row r="206" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
       <c r="G206" s="12"/>
@@ -3603,7 +3574,7 @@
       <c r="I206" s="12"/>
       <c r="J206" s="12"/>
     </row>
-    <row r="207" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E207" s="12"/>
       <c r="F207" s="12"/>
       <c r="G207" s="12"/>
@@ -3611,7 +3582,7 @@
       <c r="I207" s="12"/>
       <c r="J207" s="12"/>
     </row>
-    <row r="208" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E208" s="12"/>
       <c r="F208" s="12"/>
       <c r="G208" s="12"/>
@@ -3637,21 +3608,21 @@
   <dimension ref="B3:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3659,7 +3630,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
@@ -3667,7 +3638,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
@@ -3675,7 +3646,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>32</v>
       </c>
@@ -3683,7 +3654,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>33</v>
       </c>
@@ -3691,7 +3662,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>34</v>
       </c>
@@ -3699,7 +3670,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>35</v>
       </c>
@@ -3707,7 +3678,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>36</v>
       </c>
@@ -3715,7 +3686,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>37</v>
       </c>
@@ -3723,7 +3694,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>38</v>
       </c>
@@ -3731,7 +3702,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
@@ -3739,7 +3710,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>40</v>
       </c>
@@ -3747,7 +3718,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>41</v>
       </c>
@@ -3755,7 +3726,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>42</v>
       </c>
@@ -3763,7 +3734,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>43</v>
       </c>
@@ -3771,7 +3742,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
@@ -3779,7 +3750,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>45</v>
       </c>
@@ -3787,7 +3758,7 @@
         <v>-23.1</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>46</v>
       </c>
@@ -3795,7 +3766,7 @@
         <v>-18.600000000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>47</v>
       </c>
@@ -3803,7 +3774,7 @@
         <v>-9.4</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>48</v>
       </c>
@@ -3811,7 +3782,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
@@ -3819,7 +3790,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
@@ -3827,7 +3798,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
@@ -3835,7 +3806,7 @@
         <v>-3.2</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>52</v>
       </c>
@@ -3843,7 +3814,7 @@
         <v>-6.8</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>53</v>
       </c>
@@ -3851,7 +3822,7 @@
         <v>-7.5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>54</v>
       </c>
@@ -3859,7 +3830,7 @@
         <v>-15.5</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>55</v>
       </c>
@@ -3867,7 +3838,7 @@
         <v>-12.7</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>56</v>
       </c>
@@ -3875,7 +3846,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>57</v>
       </c>
@@ -3883,7 +3854,7 @@
         <v>-8.6</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
@@ -3891,7 +3862,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>59</v>
       </c>
@@ -3899,7 +3870,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>60</v>
       </c>
@@ -3907,7 +3878,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>61</v>
       </c>
@@ -3915,7 +3886,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>62</v>
       </c>
@@ -3923,7 +3894,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>63</v>
       </c>
@@ -3931,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>64</v>
       </c>
@@ -3939,7 +3910,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>65</v>
       </c>
@@ -3947,7 +3918,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>66</v>
       </c>
@@ -3955,7 +3926,7 @@
         <v>-6.7</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>67</v>
       </c>
@@ -3963,7 +3934,7 @@
         <v>-8.5</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>68</v>
       </c>
@@ -3971,7 +3942,7 @@
         <v>-15.7</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>69</v>
       </c>
@@ -3979,7 +3950,7 @@
         <v>-26.6</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>70</v>
       </c>
@@ -3987,7 +3958,7 @@
         <v>-26.2</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>71</v>
       </c>
@@ -3995,7 +3966,7 @@
         <v>-27.7</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>72</v>
       </c>
@@ -4003,7 +3974,7 @@
         <v>-30.9</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>73</v>
       </c>
@@ -4011,7 +3982,7 @@
         <v>-36.799999999999997</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>74</v>
       </c>
@@ -4019,7 +3990,7 @@
         <v>-42.5</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>